<commit_message>
adding create new client
</commit_message>
<xml_diff>
--- a/AutomationTestSuite/src/test/resources/data.xlsx
+++ b/AutomationTestSuite/src/test/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\AutomationTestSuite\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B090FC-8976-4019-9221-B663F3A1F1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A3ED5C-2189-4FE3-A123-93E0EAC7B181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="703" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="703" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="purchaseReturnWithoutRef" sheetId="9" r:id="rId8"/>
     <sheet name="purchaseCashback" sheetId="10" r:id="rId9"/>
     <sheet name="VatReport" sheetId="4" r:id="rId10"/>
+    <sheet name="clients" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="100">
   <si>
     <t>email</t>
   </si>
@@ -199,6 +200,141 @@
   </si>
   <si>
     <t>Jul 05 2024</t>
+  </si>
+  <si>
+    <t>shortName</t>
+  </si>
+  <si>
+    <t>accountType</t>
+  </si>
+  <si>
+    <t>relationshipType</t>
+  </si>
+  <si>
+    <t>corporateType</t>
+  </si>
+  <si>
+    <t>commercialRegistartionNo</t>
+  </si>
+  <si>
+    <t>unifiedNo</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>vatRegistrationNo</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>referenceNo</t>
+  </si>
+  <si>
+    <t>ArAddress</t>
+  </si>
+  <si>
+    <t>EnAddress</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>منة الله عماد</t>
+  </si>
+  <si>
+    <t>Menna Emad</t>
+  </si>
+  <si>
+    <t>حساب</t>
+  </si>
+  <si>
+    <t>كلاهما</t>
+  </si>
+  <si>
+    <t>مؤسسة</t>
+  </si>
+  <si>
+    <t>https://fai-wp.ahadtest.com</t>
+  </si>
+  <si>
+    <t>123451234512345</t>
+  </si>
+  <si>
+    <t>مصر</t>
+  </si>
+  <si>
+    <t>الإسكندرية</t>
+  </si>
+  <si>
+    <t>سموحه</t>
+  </si>
+  <si>
+    <t>smouha</t>
+  </si>
+  <si>
+    <t>0559505553</t>
+  </si>
+  <si>
+    <t>repArName</t>
+  </si>
+  <si>
+    <t>repEnName</t>
+  </si>
+  <si>
+    <t>ArTitle</t>
+  </si>
+  <si>
+    <t>EnTitle</t>
+  </si>
+  <si>
+    <t>ماريو نادى</t>
+  </si>
+  <si>
+    <t>مدير منتج</t>
+  </si>
+  <si>
+    <t>MarioNady</t>
+  </si>
+  <si>
+    <t>product manager</t>
+  </si>
+  <si>
+    <t>repEmail</t>
+  </si>
+  <si>
+    <t>mario@fai.ws</t>
+  </si>
+  <si>
+    <t>menna@fai.ws</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>مُعتَمَد</t>
+  </si>
+  <si>
+    <t>repPhone</t>
+  </si>
+  <si>
+    <t>0559505554</t>
   </si>
 </sst>
 </file>
@@ -618,6 +754,208 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B52009-A83D-4013-B030-64DC2CD80673}">
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="10.21875" customWidth="1"/>
+    <col min="17" max="17" width="9.5546875" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" customWidth="1"/>
+    <col min="21" max="21" width="10.77734375" customWidth="1"/>
+    <col min="23" max="23" width="15.88671875" customWidth="1"/>
+    <col min="24" max="24" width="12" customWidth="1"/>
+    <col min="26" max="26" width="11.109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W1" t="s">
+        <v>88</v>
+      </c>
+      <c r="X1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2">
+        <v>1111122222</v>
+      </c>
+      <c r="H2">
+        <v>5555566666</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2">
+        <v>123</v>
+      </c>
+      <c r="O2">
+        <v>12345</v>
+      </c>
+      <c r="P2" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="T2" t="s">
+        <v>89</v>
+      </c>
+      <c r="U2" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" t="s">
+        <v>90</v>
+      </c>
+      <c r="W2" t="s">
+        <v>92</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{D1EB1092-3E62-48FC-9719-3D01E79FC5B4}"/>
+    <hyperlink ref="S2" r:id="rId2" xr:uid="{4ABDD191-21B4-44A5-BC4B-5FA647F112A8}"/>
+    <hyperlink ref="X2" r:id="rId3" xr:uid="{BB146E7C-5CE5-401F-8131-C8ED3C802883}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0978804B-D341-4909-A367-7267DE1FF7A1}">
   <dimension ref="A1:K2"/>
@@ -989,7 +1327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CE336D-961F-47DC-9682-35235FA451C1}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding add new company class
</commit_message>
<xml_diff>
--- a/AutomationTestSuite/src/test/resources/data.xlsx
+++ b/AutomationTestSuite/src/test/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\AutomationTestSuite\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A3ED5C-2189-4FE3-A123-93E0EAC7B181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51956363-D033-44B7-804F-C0302A45B3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="703" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="703" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="purchaseCashback" sheetId="10" r:id="rId9"/>
     <sheet name="VatReport" sheetId="4" r:id="rId10"/>
     <sheet name="clients" sheetId="13" r:id="rId11"/>
+    <sheet name="company" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="118">
   <si>
     <t>email</t>
   </si>
@@ -335,6 +336,60 @@
   </si>
   <si>
     <t>0559505554</t>
+  </si>
+  <si>
+    <t>companyType</t>
+  </si>
+  <si>
+    <t>Fai</t>
+  </si>
+  <si>
+    <t>منشأة</t>
+  </si>
+  <si>
+    <t>organizationType</t>
+  </si>
+  <si>
+    <t>commercialRegistrtaionNo</t>
+  </si>
+  <si>
+    <t>taxNo</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>111112222233333</t>
+  </si>
+  <si>
+    <t>0987654321</t>
+  </si>
+  <si>
+    <t>1111122222</t>
+  </si>
+  <si>
+    <t>effectiveVATRegistrationDate</t>
+  </si>
+  <si>
+    <t>Jan 01 2024</t>
+  </si>
+  <si>
+    <t>reportType</t>
+  </si>
+  <si>
+    <t>شهري</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>Mario Nady</t>
+  </si>
+  <si>
+    <t>مالك الحساب</t>
   </si>
 </sst>
 </file>
@@ -379,10 +434,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -758,7 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B52009-A83D-4013-B030-64DC2CD80673}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
@@ -951,6 +1007,114 @@
     <hyperlink ref="I2" r:id="rId1" xr:uid="{D1EB1092-3E62-48FC-9719-3D01E79FC5B4}"/>
     <hyperlink ref="S2" r:id="rId2" xr:uid="{4ABDD191-21B4-44A5-BC4B-5FA647F112A8}"/>
     <hyperlink ref="X2" r:id="rId3" xr:uid="{BB146E7C-5CE5-401F-8131-C8ED3C802883}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53839567-F6A2-4DAF-87F5-C7A64298C766}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{41B70C04-43BE-4D1F-97EB-A7779E9B787C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1487,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494E087B-1E74-4DBF-A126-0DCB7705C97B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding create new product
</commit_message>
<xml_diff>
--- a/AutomationTestSuite/src/test/resources/data.xlsx
+++ b/AutomationTestSuite/src/test/resources/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\AutomationTestSuite\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51956363-D033-44B7-804F-C0302A45B3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A74B39-E073-4496-BA05-DAC58A61A144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="703" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="703" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="VatReport" sheetId="4" r:id="rId10"/>
     <sheet name="clients" sheetId="13" r:id="rId11"/>
     <sheet name="company" sheetId="14" r:id="rId12"/>
+    <sheet name="products" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="126">
   <si>
     <t>email</t>
   </si>
@@ -320,12 +321,6 @@
     <t>repEmail</t>
   </si>
   <si>
-    <t>mario@fai.ws</t>
-  </si>
-  <si>
-    <t>menna@fai.ws</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -390,6 +385,36 @@
   </si>
   <si>
     <t>مالك الحساب</t>
+  </si>
+  <si>
+    <t>mario@fai.sa</t>
+  </si>
+  <si>
+    <t>menna@fai.sa</t>
+  </si>
+  <si>
+    <t>منتج</t>
+  </si>
+  <si>
+    <t>ArDescription</t>
+  </si>
+  <si>
+    <t>وصف المنتج</t>
+  </si>
+  <si>
+    <t>EnDescription</t>
+  </si>
+  <si>
+    <t>product description</t>
+  </si>
+  <si>
+    <t>productType</t>
+  </si>
+  <si>
+    <t>productCode</t>
+  </si>
+  <si>
+    <t>Auto</t>
   </si>
 </sst>
 </file>
@@ -815,7 +840,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,7 +863,7 @@
     <col min="20" max="20" width="10.33203125" customWidth="1"/>
     <col min="21" max="21" width="10.77734375" customWidth="1"/>
     <col min="23" max="23" width="15.88671875" customWidth="1"/>
-    <col min="24" max="24" width="12" customWidth="1"/>
+    <col min="24" max="24" width="18.21875" customWidth="1"/>
     <col min="26" max="26" width="11.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -916,10 +941,10 @@
         <v>93</v>
       </c>
       <c r="Y1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -978,7 +1003,7 @@
         <v>84</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="T2" t="s">
         <v>89</v>
@@ -993,13 +1018,13 @@
         <v>92</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="Y2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1017,7 +1042,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1041,81 +1066,151 @@
         <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>62</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{41B70C04-43BE-4D1F-97EB-A7779E9B787C}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AFABAF-F97A-47E7-8DD6-3FE651B79F04}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1651,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494E087B-1E74-4DBF-A126-0DCB7705C97B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>